<commit_message>
comentarios para las entidades
</commit_message>
<xml_diff>
--- a/Beta_Design_Data_Base.xlsx
+++ b/Beta_Design_Data_Base.xlsx
@@ -29,6 +29,328 @@
     <author>Walter</author>
   </authors>
   <commentList>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Usuarios registrados dentro de la plataforma</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Walter:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tabla que almacenará todos y cada uno de los proyectos que se creen el la plataforma</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Listado de usuarios asignados para cada proyecto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+definira si el comentario será para proyecto, Objetivo y/o tarea</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+almacenará los comentarios que todo proyecto, objetivo y tarea pueden tener
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Son todos y cada uno de los requerimientos que tendra cada proyecto, estaran definidos por objetivos para que sean alcanzado por el equipo desigando a cada proyecto. Por ejemplo: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rediseño de Landing Page Empresarial</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+El estado del proyecto lo definira si esta iniciado, detenido y/o concluido</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+almacenará todas y cada de las tareas que sean asigandas a cada usuario por proyecto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+define el estado en que se encuentra el Objetivo del proyecto. En Espera, Aceptado, En Curso, Detenido y Finalizado</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Servirán para indicar de que tipo de tarea será, ya sea diseño, maquetado, funcionalidad, o alguna otra descripción que quieran agregar al proyecto, Objetivo o Tarea
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Son las tareas por cada objetivo que se defina dentro del proyecto, por ejemplo: Si uno de los objetivos es </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Diseño completo del nuevo landing page empresarial</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, un listado de las tareas sería:
+1. Definir nuevos colores para landing Page.
+2. Definir nuevos textos y call to actions.
+3. Diseñar nueva UX | UI para landing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Define el nivel de prioridad de cada Objetivo o Tarea, puede ser: norma, media, alta</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G39" authorId="0" shapeId="0">
       <text>
         <r>
@@ -50,6 +372,31 @@
           </rPr>
           <t xml:space="preserve">
 considerando si este tabla sera para ser publico, privado.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K39" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Almacenará imágenes y/o documentos que tengan información relacionada con la tarea y que deseen agregar como información adicional para la tarea
 </t>
         </r>
       </text>
@@ -75,6 +422,54 @@
           </rPr>
           <t xml:space="preserve">
 Indica si el objetivo sera personal, departamental o institucional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+almacenará el listado de reconocimientos que cada usuario tenga</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Son todos y cada uno de los reconocimientos con los que contará la plataforma para reconocer a los colaboradores, tales como: pasion por su trabajo, trabajo en equipo, etc.</t>
         </r>
       </text>
     </comment>
@@ -380,7 +775,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +803,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -482,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,6 +901,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,6 +1330,7 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
+      <c r="C9" s="10"/>
       <c r="E9" s="6" t="s">
         <v>63</v>
       </c>
@@ -941,6 +1348,7 @@
       <c r="A10" t="s">
         <v>26</v>
       </c>
+      <c r="C10" s="11"/>
       <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
@@ -958,6 +1366,7 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
+      <c r="C11" s="11"/>
       <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
@@ -975,6 +1384,7 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
+      <c r="C12" s="11"/>
       <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
@@ -992,6 +1402,7 @@
       <c r="A13" t="s">
         <v>29</v>
       </c>
+      <c r="C13" s="11"/>
       <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1003,6 +1414,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="11"/>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1017,6 +1429,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="11"/>
       <c r="E15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1031,6 +1444,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="11"/>
       <c r="E16" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
cambios en estructura Beta
</commit_message>
<xml_diff>
--- a/Beta_Design_Data_Base.xlsx
+++ b/Beta_Design_Data_Base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\PROYECTOS\PMS OKRS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\weredone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -61,7 +61,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Walter:
 </t>
@@ -184,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="0" shapeId="0">
+    <comment ref="E18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -204,11 +204,36 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-El estado del proyecto lo definira si esta iniciado, detenido y/o concluido</t>
+Guardará todos los objetos para los respectivos estados, Proyecto, Objetivos, Tareas, Inconvenientes
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="G18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+La tabla estados generales definirá todos y cada uno de los estados que podrá contener tanto los proyectos, como objetivos y las tareas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G27" authorId="0" shapeId="0">
+    <comment ref="G25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -252,11 +277,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-define el estado en que se encuentra el Objetivo del proyecto. En Espera, Aceptado, En Curso, Detenido y Finalizado</t>
+Define el nivel de prioridad de cada Objetivo o Tarea, puede ser: norma, media, alta</t>
         </r>
       </text>
     </comment>
-    <comment ref="K28" authorId="0" shapeId="0">
+    <comment ref="K26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -277,6 +302,31 @@
           </rPr>
           <t xml:space="preserve">
 Servirán para indicar de que tipo de tarea será, ya sea diseño, maquetado, funcionalidad, o alguna otra descripción que quieran agregar al proyecto, Objetivo o Tarea
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+considerando si este tabla sera para ser publico, privado.
 </t>
         </r>
       </text>
@@ -327,56 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Walter:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Define el nivel de prioridad de cada Objetivo o Tarea, puede ser: norma, media, alta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G39" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Walter:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-considerando si este tabla sera para ser publico, privado.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K39" authorId="0" shapeId="0">
+    <comment ref="K35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -401,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G45" authorId="0" shapeId="0">
+    <comment ref="G37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,6 +423,30 @@
           </rPr>
           <t xml:space="preserve">
 Indica si el objetivo sera personal, departamental o institucional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G43" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Walter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Son todos y cada uno de los reconocimientos con los que contará la plataforma para reconocer a los colaboradores, tales como: pasion por su trabajo, trabajo en equipo, etc.</t>
         </r>
       </text>
     </comment>
@@ -446,30 +471,6 @@
           </rPr>
           <t xml:space="preserve">
 almacenará el listado de reconocimientos que cada usuario tenga</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Walter:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Son todos y cada uno de los reconocimientos con los que contará la plataforma para reconocer a los colaboradores, tales como: pasion por su trabajo, trabajo en equipo, etc.</t>
         </r>
       </text>
     </comment>
@@ -478,7 +479,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
   <si>
     <t>PROYECTO PMS</t>
   </si>
@@ -537,9 +538,6 @@
     <t>idAdministrador:int</t>
   </si>
   <si>
-    <t>descripcion:varchar(100)</t>
-  </si>
-  <si>
     <t>nombreProyecto:varchar(100)</t>
   </si>
   <si>
@@ -579,15 +577,6 @@
     <t>porcentajeAvance: float</t>
   </si>
   <si>
-    <t>Atrasos: int</t>
-  </si>
-  <si>
-    <t>Problemas: int</t>
-  </si>
-  <si>
-    <t>Objetivos: int</t>
-  </si>
-  <si>
     <t>crearProyecto()</t>
   </si>
   <si>
@@ -603,9 +592,6 @@
     <t>cambiarEstadoProyecto(idStatus)</t>
   </si>
   <si>
-    <t>estadosProyecto</t>
-  </si>
-  <si>
     <t>idEstadoProyecto: int</t>
   </si>
   <si>
@@ -651,9 +637,6 @@
     <t>descripcion: varchar(100)</t>
   </si>
   <si>
-    <t>EstadoObjetivo</t>
-  </si>
-  <si>
     <t>idEstadoObjetivo: int</t>
   </si>
   <si>
@@ -717,9 +700,6 @@
     <t>idTipoComentario: int</t>
   </si>
   <si>
-    <t>idObjetivo: int</t>
-  </si>
-  <si>
     <t>idTareaObjetivo: int</t>
   </si>
   <si>
@@ -769,13 +749,46 @@
   </si>
   <si>
     <t>idClaseObjetivo: int</t>
+  </si>
+  <si>
+    <t>idTipoInconveniente: int</t>
+  </si>
+  <si>
+    <t>idUsuarioReporta: int</t>
+  </si>
+  <si>
+    <t>Descripcion: varchar(250)</t>
+  </si>
+  <si>
+    <t>fechaReporte: datetime</t>
+  </si>
+  <si>
+    <t>fechaSolucion: datetime</t>
+  </si>
+  <si>
+    <t>estadoInconveniente: int</t>
+  </si>
+  <si>
+    <t>tipoInconveniente</t>
+  </si>
+  <si>
+    <t>estadosGenerales</t>
+  </si>
+  <si>
+    <t>idTipoObjeto: int</t>
+  </si>
+  <si>
+    <t>TipoObjeto</t>
+  </si>
+  <si>
+    <t>Inconvenientes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,13 +816,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -884,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -898,9 +904,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1200,7 @@
     <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" customWidth="1"/>
@@ -1205,16 +1208,17 @@
     <col min="10" max="10" width="3.140625" customWidth="1"/>
     <col min="11" max="11" width="26.28515625" customWidth="1"/>
     <col min="12" max="12" width="3.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -1226,13 +1230,16 @@
         <v>17</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1251,10 +1258,13 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
@@ -1266,15 +1276,18 @@
         <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1283,18 +1296,21 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
@@ -1303,57 +1319,66 @@
         <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="E9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>35</v>
+        <v>57</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="C10" s="10"/>
       <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>5</v>
@@ -1361,457 +1386,463 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="C11" s="10"/>
       <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>33</v>
+      <c r="G11" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="C12" s="10"/>
       <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>43</v>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="C13" s="10"/>
       <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="11"/>
+        <v>98</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C14" s="10"/>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>4</v>
+      <c r="G14" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="10"/>
       <c r="E15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>36</v>
+      <c r="G15" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="11"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="10"/>
       <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>37</v>
+      <c r="G16" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G24" s="9"/>
+      <c r="I24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K17" s="3" t="s">
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="K18" s="4" t="s">
+      <c r="K27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G28" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I20" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G28" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="3" t="s">
-        <v>56</v>
+      <c r="K28" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G29" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="4" t="s">
+      <c r="I32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="1" t="s">
-        <v>61</v>
+      <c r="G33" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K34" s="3" t="s">
+    <row r="39" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G39" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G37" s="5" t="s">
+    </row>
+    <row r="40" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K40" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K37" s="5" t="s">
+    </row>
+    <row r="41" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G41" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="I38" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G41" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="I41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G42" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="I42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G43" s="5" t="s">
-        <v>5</v>
+      <c r="G43" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="44" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="I44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K44" s="5" t="s">
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G46" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G47" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G46" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G47" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="I47" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G48" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="I48" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I52" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="3" t="s">
-        <v>62</v>
-      </c>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I53" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>